<commit_message>
trying to tidy data and run first sets of models for lichem, coral, and algae
</commit_message>
<xml_diff>
--- a/wos155_screenabs3july2023.xlsx
+++ b/wos155_screenabs3july2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretslein/lichen/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2C929B-564A-F043-A194-49BD0AC375FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F0DDF5-6044-974E-AE1E-9507DD66E926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="520" windowWidth="19400" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3640" yWindow="1080" windowWidth="20880" windowHeight="12100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wos155_screenabs20oct21" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4122" uniqueCount="1667">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4123" uniqueCount="1668">
   <si>
     <t>label</t>
   </si>
@@ -5036,6 +5036,9 @@
   </si>
   <si>
     <t>figure 6</t>
+  </si>
+  <si>
+    <t>kappen1983</t>
   </si>
 </sst>
 </file>
@@ -5555,7 +5558,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -5566,8 +5569,6 @@
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5925,10 +5926,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH156"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="O1" sqref="O1"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6132,2795 +6133,2795 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="3" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3">
         <v>2005</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3">
         <v>142</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="1">
         <v>45249</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" t="s">
         <v>52</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" t="s">
         <v>54</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="10" t="s">
+      <c r="O3" t="s">
         <v>55</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y3" s="10" t="s">
+      <c r="P3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>45</v>
+      </c>
+      <c r="R3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S3" t="s">
+        <v>45</v>
+      </c>
+      <c r="T3" t="s">
+        <v>45</v>
+      </c>
+      <c r="U3" t="s">
+        <v>45</v>
+      </c>
+      <c r="V3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" t="s">
         <v>46</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="Z3" t="s">
         <v>56</v>
       </c>
-      <c r="AA3" s="10" t="s">
+      <c r="AA3" t="s">
         <v>48</v>
       </c>
-      <c r="AB3" s="10" t="s">
+      <c r="AB3" t="s">
         <v>48</v>
       </c>
-      <c r="AC3" s="10" t="s">
+      <c r="AC3" t="s">
         <v>57</v>
       </c>
-      <c r="AD3" s="10" t="s">
+      <c r="AD3" t="s">
         <v>48</v>
       </c>
-      <c r="AE3" s="10" t="s">
+      <c r="AE3" t="s">
         <v>58</v>
       </c>
-      <c r="AF3" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG3" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH3" s="10" t="s">
+      <c r="AF3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" t="s">
         <v>62</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4">
         <v>2019</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4">
         <v>12</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4">
         <v>4</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" t="s">
         <v>64</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" t="s">
         <v>65</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" t="s">
         <v>66</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="M4" t="s">
         <v>67</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" t="s">
         <v>68</v>
       </c>
-      <c r="O4" s="10" t="s">
+      <c r="O4" t="s">
         <v>69</v>
       </c>
-      <c r="P4" s="10" t="s">
+      <c r="P4" t="s">
         <v>70</v>
       </c>
-      <c r="Q4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X4" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Q4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" t="s">
+        <v>45</v>
+      </c>
+      <c r="S4" t="s">
+        <v>45</v>
+      </c>
+      <c r="T4" t="s">
+        <v>45</v>
+      </c>
+      <c r="U4" t="s">
+        <v>45</v>
+      </c>
+      <c r="V4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W4" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y4" t="s">
         <v>46</v>
       </c>
-      <c r="Z4" s="10" t="s">
+      <c r="Z4" t="s">
         <v>71</v>
       </c>
-      <c r="AA4" s="10" t="s">
+      <c r="AA4" t="s">
         <v>48</v>
       </c>
-      <c r="AB4" s="10" t="s">
+      <c r="AB4" t="s">
         <v>48</v>
       </c>
-      <c r="AC4" s="10" t="s">
+      <c r="AC4" t="s">
         <v>72</v>
       </c>
-      <c r="AD4" s="10" t="s">
+      <c r="AD4" t="s">
         <v>48</v>
       </c>
-      <c r="AF4" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG4" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH4" s="10" t="s">
+      <c r="AF4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" t="s">
         <v>74</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" t="s">
         <v>75</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" t="s">
         <v>76</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5">
         <v>2020</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5">
         <v>43</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5">
         <v>12</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" t="s">
         <v>78</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" t="s">
         <v>79</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" t="s">
         <v>80</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" t="s">
         <v>81</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" t="s">
         <v>82</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" t="s">
         <v>83</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" t="s">
         <v>84</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" t="s">
         <v>85</v>
       </c>
-      <c r="R5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X5" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y5" s="10" t="s">
+      <c r="R5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T5" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" t="s">
+        <v>45</v>
+      </c>
+      <c r="V5" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y5" t="s">
         <v>46</v>
       </c>
-      <c r="Z5" s="10" t="s">
+      <c r="Z5" t="s">
         <v>86</v>
       </c>
-      <c r="AA5" s="10" t="s">
+      <c r="AA5" t="s">
         <v>48</v>
       </c>
-      <c r="AB5" s="10" t="s">
+      <c r="AB5" t="s">
         <v>48</v>
       </c>
-      <c r="AC5" s="10" t="s">
+      <c r="AC5" t="s">
         <v>87</v>
       </c>
-      <c r="AD5" s="10" t="s">
+      <c r="AD5" t="s">
         <v>48</v>
       </c>
-      <c r="AE5" s="10" t="s">
+      <c r="AE5" t="s">
         <v>88</v>
       </c>
-      <c r="AF5" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG5" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH5" s="10" t="s">
+      <c r="AF5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG5" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" t="s">
         <v>90</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6">
         <v>2018</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6">
         <v>24</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6">
         <v>3</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" t="s">
         <v>94</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" t="s">
         <v>95</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" t="s">
         <v>96</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" t="s">
         <v>97</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" t="s">
         <v>98</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" t="s">
         <v>99</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" t="s">
         <v>100</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="Q6" t="s">
         <v>101</v>
       </c>
-      <c r="R6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X6" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y6" s="10" t="s">
+      <c r="R6" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" t="s">
+        <v>45</v>
+      </c>
+      <c r="T6" t="s">
+        <v>45</v>
+      </c>
+      <c r="U6" t="s">
+        <v>45</v>
+      </c>
+      <c r="V6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" t="s">
+        <v>45</v>
+      </c>
+      <c r="X6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y6" t="s">
         <v>46</v>
       </c>
-      <c r="Z6" s="10" t="s">
+      <c r="Z6" t="s">
         <v>86</v>
       </c>
-      <c r="AA6" s="10" t="s">
+      <c r="AA6" t="s">
         <v>48</v>
       </c>
-      <c r="AB6" s="10" t="s">
+      <c r="AB6" t="s">
         <v>48</v>
       </c>
-      <c r="AC6" s="10" t="s">
+      <c r="AC6" t="s">
         <v>102</v>
       </c>
-      <c r="AD6" s="10" t="s">
+      <c r="AD6" t="s">
         <v>48</v>
       </c>
-      <c r="AE6" s="10" t="s">
+      <c r="AE6" t="s">
         <v>103</v>
       </c>
-      <c r="AF6" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG6" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH6" s="10" t="s">
+      <c r="AF6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" t="s">
         <v>106</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" t="s">
         <v>107</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7">
         <v>1999</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7">
         <v>13</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7">
         <v>1</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" t="s">
         <v>108</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" t="s">
         <v>109</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" t="s">
         <v>110</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" t="s">
         <v>111</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" t="s">
         <v>112</v>
       </c>
-      <c r="N7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="10" t="s">
+      <c r="N7" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" t="s">
         <v>113</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" t="s">
         <v>114</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" t="s">
         <v>115</v>
       </c>
-      <c r="R7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y7" s="10" t="s">
+      <c r="R7" t="s">
+        <v>45</v>
+      </c>
+      <c r="S7" t="s">
+        <v>45</v>
+      </c>
+      <c r="T7" t="s">
+        <v>45</v>
+      </c>
+      <c r="U7" t="s">
+        <v>45</v>
+      </c>
+      <c r="V7" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" t="s">
+        <v>45</v>
+      </c>
+      <c r="X7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y7" t="s">
         <v>46</v>
       </c>
-      <c r="Z7" s="10" t="s">
+      <c r="Z7" t="s">
         <v>71</v>
       </c>
-      <c r="AA7" s="10" t="s">
+      <c r="AA7" t="s">
         <v>48</v>
       </c>
-      <c r="AB7" s="10" t="s">
+      <c r="AB7" t="s">
         <v>48</v>
       </c>
-      <c r="AC7" s="10" t="s">
+      <c r="AC7" t="s">
         <v>57</v>
       </c>
-      <c r="AD7" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE7" s="10" t="s">
+      <c r="AD7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE7" t="s">
         <v>1636</v>
       </c>
-      <c r="AF7" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG7" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH7" s="10" t="s">
+      <c r="AF7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG7" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH7" t="s">
         <v>1607</v>
       </c>
     </row>
-    <row r="8" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>117</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" t="s">
         <v>118</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" t="s">
         <v>120</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8">
         <v>1995</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8">
         <v>131</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8">
         <v>2</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" t="s">
         <v>121</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" t="s">
         <v>122</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" t="s">
         <v>123</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" t="s">
         <v>124</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" t="s">
         <v>125</v>
       </c>
-      <c r="N8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O8" s="10" t="s">
+      <c r="N8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" t="s">
         <v>126</v>
       </c>
-      <c r="P8" s="10" t="s">
+      <c r="P8" t="s">
         <v>127</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="Q8" t="s">
         <v>128</v>
       </c>
-      <c r="R8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y8" s="10" t="s">
+      <c r="R8" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" t="s">
+        <v>45</v>
+      </c>
+      <c r="T8" t="s">
+        <v>45</v>
+      </c>
+      <c r="U8" t="s">
+        <v>45</v>
+      </c>
+      <c r="V8" t="s">
+        <v>45</v>
+      </c>
+      <c r="W8" t="s">
+        <v>45</v>
+      </c>
+      <c r="X8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y8" t="s">
         <v>46</v>
       </c>
-      <c r="AA8" s="10" t="s">
+      <c r="AA8" t="s">
         <v>48</v>
       </c>
-      <c r="AB8" s="10" t="s">
+      <c r="AB8" t="s">
         <v>48</v>
       </c>
-      <c r="AC8" s="10" t="s">
+      <c r="AC8" t="s">
         <v>87</v>
       </c>
-      <c r="AD8" s="10" t="s">
+      <c r="AD8" t="s">
         <v>48</v>
       </c>
-      <c r="AE8" s="10" t="s">
+      <c r="AE8" t="s">
         <v>129</v>
       </c>
-      <c r="AF8" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG8" s="10" t="s">
+      <c r="AF8" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG8" t="s">
         <v>48</v>
       </c>
-      <c r="AH8" s="10" t="s">
+      <c r="AH8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>130</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" t="s">
         <v>132</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9">
         <v>2001</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9">
         <v>149</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" t="s">
         <v>133</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" t="s">
         <v>109</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" t="s">
         <v>134</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" t="s">
         <v>135</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="M9" t="s">
         <v>125</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" t="s">
         <v>136</v>
       </c>
-      <c r="O9" s="10" t="s">
+      <c r="O9" t="s">
         <v>137</v>
       </c>
-      <c r="P9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y9" s="10" t="s">
+      <c r="P9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>45</v>
+      </c>
+      <c r="R9" t="s">
+        <v>45</v>
+      </c>
+      <c r="S9" t="s">
+        <v>45</v>
+      </c>
+      <c r="T9" t="s">
+        <v>45</v>
+      </c>
+      <c r="U9" t="s">
+        <v>45</v>
+      </c>
+      <c r="V9" t="s">
+        <v>45</v>
+      </c>
+      <c r="W9" t="s">
+        <v>45</v>
+      </c>
+      <c r="X9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y9" t="s">
         <v>46</v>
       </c>
-      <c r="Z9" s="10" t="s">
+      <c r="Z9" t="s">
         <v>138</v>
       </c>
-      <c r="AA9" s="10" t="s">
+      <c r="AA9" t="s">
         <v>48</v>
       </c>
-      <c r="AB9" s="10" t="s">
+      <c r="AB9" t="s">
         <v>48</v>
       </c>
-      <c r="AC9" s="10" t="s">
+      <c r="AC9" t="s">
         <v>57</v>
       </c>
-      <c r="AD9" s="10" t="s">
+      <c r="AD9" t="s">
         <v>48</v>
       </c>
-      <c r="AE9" s="10" t="s">
+      <c r="AE9" t="s">
         <v>1628</v>
       </c>
-      <c r="AF9" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG9" s="10" t="s">
+      <c r="AF9" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG9" t="s">
         <v>48</v>
       </c>
-      <c r="AH9" s="10" t="s">
+      <c r="AH9" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" t="s">
         <v>140</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" t="s">
         <v>141</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" t="s">
         <v>142</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10">
         <v>2002</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10">
         <v>197</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10">
         <v>4</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" t="s">
         <v>143</v>
       </c>
-      <c r="J10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" s="10" t="s">
+      <c r="J10" t="s">
+        <v>45</v>
+      </c>
+      <c r="K10" t="s">
         <v>144</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" t="s">
         <v>145</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" t="s">
         <v>146</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" t="s">
         <v>147</v>
       </c>
-      <c r="O10" s="10" t="s">
+      <c r="O10" t="s">
         <v>148</v>
       </c>
-      <c r="P10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y10" s="10" t="s">
+      <c r="P10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>45</v>
+      </c>
+      <c r="R10" t="s">
+        <v>45</v>
+      </c>
+      <c r="S10" t="s">
+        <v>45</v>
+      </c>
+      <c r="T10" t="s">
+        <v>45</v>
+      </c>
+      <c r="U10" t="s">
+        <v>45</v>
+      </c>
+      <c r="V10" t="s">
+        <v>45</v>
+      </c>
+      <c r="W10" t="s">
+        <v>45</v>
+      </c>
+      <c r="X10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y10" t="s">
         <v>46</v>
       </c>
-      <c r="AA10" s="10" t="s">
+      <c r="AA10" t="s">
         <v>48</v>
       </c>
-      <c r="AB10" s="10" t="s">
+      <c r="AB10" t="s">
         <v>48</v>
       </c>
-      <c r="AC10" s="10" t="s">
+      <c r="AC10" t="s">
         <v>1630</v>
       </c>
-      <c r="AD10" s="10" t="s">
+      <c r="AD10" t="s">
         <v>48</v>
       </c>
-      <c r="AE10" s="10" t="s">
+      <c r="AE10" t="s">
         <v>1605</v>
       </c>
-      <c r="AF10" s="10" t="s">
+      <c r="AF10" t="s">
         <v>48</v>
       </c>
-      <c r="AG10" s="10" t="s">
+      <c r="AG10" t="s">
         <v>48</v>
       </c>
-      <c r="AH10" s="10" t="s">
+      <c r="AH10" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>149</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" t="s">
         <v>150</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" t="s">
         <v>151</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11">
         <v>2000</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11">
         <v>195</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" t="s">
         <v>152</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K11" t="s">
         <v>153</v>
       </c>
-      <c r="L11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="M11" s="10" t="s">
+      <c r="L11" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" t="s">
         <v>146</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" t="s">
         <v>147</v>
       </c>
-      <c r="O11" s="10" t="s">
+      <c r="O11" t="s">
         <v>154</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="P11" t="s">
         <v>155</v>
       </c>
-      <c r="Q11" s="10" t="s">
+      <c r="Q11" t="s">
         <v>156</v>
       </c>
-      <c r="R11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X11" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y11" s="10" t="s">
+      <c r="R11" t="s">
+        <v>45</v>
+      </c>
+      <c r="S11" t="s">
+        <v>45</v>
+      </c>
+      <c r="T11" t="s">
+        <v>45</v>
+      </c>
+      <c r="U11" t="s">
+        <v>45</v>
+      </c>
+      <c r="V11" t="s">
+        <v>45</v>
+      </c>
+      <c r="W11" t="s">
+        <v>45</v>
+      </c>
+      <c r="X11" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y11" t="s">
         <v>46</v>
       </c>
-      <c r="AA11" s="10" t="s">
+      <c r="AA11" t="s">
         <v>48</v>
       </c>
-      <c r="AB11" s="10" t="s">
+      <c r="AB11" t="s">
         <v>48</v>
       </c>
-      <c r="AC11" s="10" t="s">
+      <c r="AC11" t="s">
         <v>157</v>
       </c>
-      <c r="AD11" s="10" t="s">
+      <c r="AD11" t="s">
         <v>48</v>
       </c>
-      <c r="AE11" s="10" t="s">
+      <c r="AE11" t="s">
         <v>158</v>
       </c>
-      <c r="AF11" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG11" s="10" t="s">
+      <c r="AF11" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG11" t="s">
         <v>48</v>
       </c>
-      <c r="AH11" s="10" t="s">
+      <c r="AH11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" t="s">
         <v>160</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" t="s">
         <v>161</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" t="s">
         <v>162</v>
       </c>
-      <c r="F12" s="10">
+      <c r="F12">
         <v>2007</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12">
         <v>226</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12">
         <v>5</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" t="s">
         <v>163</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" t="s">
         <v>122</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K12" t="s">
         <v>164</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" t="s">
         <v>165</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" t="s">
         <v>166</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="N12" t="s">
         <v>167</v>
       </c>
-      <c r="O12" s="10" t="s">
+      <c r="O12" t="s">
         <v>168</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="P12" t="s">
         <v>169</v>
       </c>
-      <c r="Q12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X12" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y12" s="10" t="s">
+      <c r="Q12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R12" t="s">
+        <v>45</v>
+      </c>
+      <c r="S12" t="s">
+        <v>45</v>
+      </c>
+      <c r="T12" t="s">
+        <v>45</v>
+      </c>
+      <c r="U12" t="s">
+        <v>45</v>
+      </c>
+      <c r="V12" t="s">
+        <v>45</v>
+      </c>
+      <c r="W12" t="s">
+        <v>45</v>
+      </c>
+      <c r="X12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y12" t="s">
         <v>46</v>
       </c>
-      <c r="AA12" s="10" t="s">
+      <c r="AA12" t="s">
         <v>48</v>
       </c>
-      <c r="AB12" s="10" t="s">
+      <c r="AB12" t="s">
         <v>48</v>
       </c>
-      <c r="AC12" s="10" t="s">
+      <c r="AC12" t="s">
         <v>87</v>
       </c>
-      <c r="AD12" s="10" t="s">
+      <c r="AD12" t="s">
         <v>48</v>
       </c>
-      <c r="AF12" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG12" s="10" t="s">
+      <c r="AF12" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG12" t="s">
         <v>48</v>
       </c>
-      <c r="AH12" s="10" t="s">
+      <c r="AH12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>170</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" t="s">
         <v>171</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" t="s">
         <v>172</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" t="s">
         <v>173</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13">
         <v>2000</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13">
         <v>12</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13">
         <v>3</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" t="s">
         <v>174</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" t="s">
         <v>175</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" t="s">
         <v>176</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" t="s">
         <v>177</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="M13" t="s">
         <v>178</v>
       </c>
-      <c r="N13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O13" s="10" t="s">
+      <c r="N13" t="s">
+        <v>45</v>
+      </c>
+      <c r="O13" t="s">
         <v>179</v>
       </c>
-      <c r="P13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R13" s="10" t="s">
+      <c r="P13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>45</v>
+      </c>
+      <c r="R13" t="s">
         <v>180</v>
       </c>
-      <c r="S13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y13" s="10" t="s">
+      <c r="S13" t="s">
+        <v>45</v>
+      </c>
+      <c r="T13" t="s">
+        <v>45</v>
+      </c>
+      <c r="U13" t="s">
+        <v>45</v>
+      </c>
+      <c r="V13" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13" t="s">
+        <v>45</v>
+      </c>
+      <c r="X13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y13" t="s">
         <v>46</v>
       </c>
-      <c r="Z13" s="10" t="s">
+      <c r="Z13" t="s">
         <v>181</v>
       </c>
-      <c r="AA13" s="10" t="s">
+      <c r="AA13" t="s">
         <v>48</v>
       </c>
-      <c r="AB13" s="10" t="s">
+      <c r="AB13" t="s">
         <v>48</v>
       </c>
-      <c r="AC13" s="10" t="s">
+      <c r="AC13" t="s">
         <v>182</v>
       </c>
-      <c r="AD13" s="10" t="s">
+      <c r="AD13" t="s">
         <v>48</v>
       </c>
-      <c r="AF13" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG13" s="10" t="s">
+      <c r="AF13" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG13" t="s">
         <v>48</v>
       </c>
-      <c r="AH13" s="10" t="s">
+      <c r="AH13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>183</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" t="s">
         <v>184</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" t="s">
         <v>185</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14">
         <v>2013</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14">
         <v>173</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14">
         <v>3</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" t="s">
         <v>186</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" t="s">
         <v>37</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" t="s">
         <v>187</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" t="s">
         <v>188</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="M14" t="s">
         <v>40</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="N14" t="s">
         <v>41</v>
       </c>
-      <c r="O14" s="10" t="s">
+      <c r="O14" t="s">
         <v>189</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="P14" t="s">
         <v>190</v>
       </c>
-      <c r="Q14" s="10" t="s">
+      <c r="Q14" t="s">
         <v>191</v>
       </c>
-      <c r="R14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y14" s="10" t="s">
+      <c r="R14" t="s">
+        <v>45</v>
+      </c>
+      <c r="S14" t="s">
+        <v>45</v>
+      </c>
+      <c r="T14" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14" t="s">
+        <v>45</v>
+      </c>
+      <c r="V14" t="s">
+        <v>45</v>
+      </c>
+      <c r="W14" t="s">
+        <v>45</v>
+      </c>
+      <c r="X14" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y14" t="s">
         <v>46</v>
       </c>
-      <c r="Z14" s="10" t="s">
+      <c r="Z14" t="s">
         <v>192</v>
       </c>
-      <c r="AA14" s="10" t="s">
+      <c r="AA14" t="s">
         <v>48</v>
       </c>
-      <c r="AB14" s="10" t="s">
+      <c r="AB14" t="s">
         <v>48</v>
       </c>
-      <c r="AC14" s="10" t="s">
+      <c r="AC14" t="s">
         <v>87</v>
       </c>
-      <c r="AD14" s="10" t="s">
+      <c r="AD14" t="s">
         <v>48</v>
       </c>
-      <c r="AF14" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG14" s="10" t="s">
+      <c r="AF14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG14" t="s">
         <v>48</v>
       </c>
-      <c r="AH14" s="10" t="s">
+      <c r="AH14" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>193</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" t="s">
         <v>194</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" t="s">
         <v>195</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" t="s">
         <v>162</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15">
         <v>1998</v>
       </c>
-      <c r="G15" s="10">
+      <c r="G15">
         <v>206</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15">
         <v>4</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" t="s">
         <v>196</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" t="s">
         <v>37</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="K15" t="s">
         <v>197</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" t="s">
         <v>198</v>
       </c>
-      <c r="M15" s="10" t="s">
+      <c r="M15" t="s">
         <v>166</v>
       </c>
-      <c r="N15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O15" s="10" t="s">
+      <c r="N15" t="s">
+        <v>45</v>
+      </c>
+      <c r="O15" t="s">
         <v>199</v>
       </c>
-      <c r="P15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y15" s="10" t="s">
+      <c r="P15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>45</v>
+      </c>
+      <c r="R15" t="s">
+        <v>45</v>
+      </c>
+      <c r="S15" t="s">
+        <v>45</v>
+      </c>
+      <c r="T15" t="s">
+        <v>45</v>
+      </c>
+      <c r="U15" t="s">
+        <v>45</v>
+      </c>
+      <c r="V15" t="s">
+        <v>45</v>
+      </c>
+      <c r="W15" t="s">
+        <v>45</v>
+      </c>
+      <c r="X15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y15" t="s">
         <v>46</v>
       </c>
-      <c r="Z15" s="10" t="s">
+      <c r="Z15" t="s">
         <v>200</v>
       </c>
-      <c r="AA15" s="10" t="s">
+      <c r="AA15" t="s">
         <v>48</v>
       </c>
-      <c r="AB15" s="10" t="s">
+      <c r="AB15" t="s">
         <v>48</v>
       </c>
-      <c r="AC15" s="10" t="s">
+      <c r="AC15" t="s">
         <v>201</v>
       </c>
-      <c r="AD15" s="10" t="s">
+      <c r="AD15" t="s">
         <v>48</v>
       </c>
-      <c r="AF15" s="10" t="s">
+      <c r="AF15" t="s">
         <v>48</v>
       </c>
-      <c r="AG15" s="10" t="s">
+      <c r="AG15" t="s">
         <v>48</v>
       </c>
-      <c r="AH15" s="10" t="s">
+      <c r="AH15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>202</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" t="s">
         <v>203</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" t="s">
         <v>204</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" t="s">
         <v>205</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16">
         <v>2013</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16">
         <v>111</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16">
         <v>3</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" t="s">
         <v>206</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" t="s">
         <v>94</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K16" t="s">
         <v>207</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="L16" t="s">
         <v>208</v>
       </c>
-      <c r="M16" s="10" t="s">
+      <c r="M16" t="s">
         <v>209</v>
       </c>
-      <c r="N16" s="10" t="s">
+      <c r="N16" t="s">
         <v>210</v>
       </c>
-      <c r="O16" s="10" t="s">
+      <c r="O16" t="s">
         <v>211</v>
       </c>
-      <c r="P16" s="10" t="s">
+      <c r="P16" t="s">
         <v>212</v>
       </c>
-      <c r="Q16" s="10" t="s">
+      <c r="Q16" t="s">
         <v>213</v>
       </c>
-      <c r="R16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X16" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y16" s="10" t="s">
+      <c r="R16" t="s">
+        <v>45</v>
+      </c>
+      <c r="S16" t="s">
+        <v>45</v>
+      </c>
+      <c r="T16" t="s">
+        <v>45</v>
+      </c>
+      <c r="U16" t="s">
+        <v>45</v>
+      </c>
+      <c r="V16" t="s">
+        <v>45</v>
+      </c>
+      <c r="W16" t="s">
+        <v>45</v>
+      </c>
+      <c r="X16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y16" t="s">
         <v>46</v>
       </c>
-      <c r="AA16" s="10" t="s">
+      <c r="AA16" t="s">
         <v>48</v>
       </c>
-      <c r="AB16" s="10" t="s">
+      <c r="AB16" t="s">
         <v>48</v>
       </c>
-      <c r="AC16" s="10" t="s">
+      <c r="AC16" t="s">
         <v>102</v>
       </c>
-      <c r="AD16" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE16" s="10" t="s">
+      <c r="AD16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE16" t="s">
         <v>1631</v>
       </c>
     </row>
-    <row r="17" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>214</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" t="s">
         <v>215</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" t="s">
         <v>216</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" t="s">
         <v>35</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17">
         <v>1997</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17">
         <v>109</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="1">
         <v>45217</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" t="s">
         <v>52</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K17" t="s">
         <v>217</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="L17" t="s">
         <v>218</v>
       </c>
-      <c r="M17" s="10" t="s">
+      <c r="M17" t="s">
         <v>40</v>
       </c>
-      <c r="N17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O17" s="10" t="s">
+      <c r="N17" t="s">
+        <v>45</v>
+      </c>
+      <c r="O17" t="s">
         <v>219</v>
       </c>
-      <c r="P17" s="10" t="s">
+      <c r="P17" t="s">
         <v>220</v>
       </c>
-      <c r="Q17" s="10" t="s">
+      <c r="Q17" t="s">
         <v>221</v>
       </c>
-      <c r="R17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X17" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y17" s="10" t="s">
+      <c r="R17" t="s">
+        <v>45</v>
+      </c>
+      <c r="S17" t="s">
+        <v>45</v>
+      </c>
+      <c r="T17" t="s">
+        <v>45</v>
+      </c>
+      <c r="U17" t="s">
+        <v>45</v>
+      </c>
+      <c r="V17" t="s">
+        <v>45</v>
+      </c>
+      <c r="W17" t="s">
+        <v>45</v>
+      </c>
+      <c r="X17" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y17" t="s">
         <v>46</v>
       </c>
-      <c r="AA17" s="10" t="s">
+      <c r="AA17" t="s">
         <v>48</v>
       </c>
-      <c r="AB17" s="10" t="s">
+      <c r="AB17" t="s">
         <v>48</v>
       </c>
-      <c r="AC17" s="10" t="s">
+      <c r="AC17" t="s">
         <v>222</v>
       </c>
-      <c r="AD17" s="10" t="s">
+      <c r="AD17" t="s">
         <v>48</v>
       </c>
-      <c r="AF17" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG17" s="10" t="s">
+      <c r="AF17" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG17" t="s">
         <v>48</v>
       </c>
-      <c r="AH17" s="10" t="s">
+      <c r="AH17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>223</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" t="s">
         <v>224</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" t="s">
         <v>225</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18">
         <v>1997</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18">
         <v>111</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18">
         <v>4</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" t="s">
         <v>226</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" t="s">
         <v>227</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K18" t="s">
         <v>228</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L18" t="s">
         <v>229</v>
       </c>
-      <c r="M18" s="10" t="s">
+      <c r="M18" t="s">
         <v>40</v>
       </c>
-      <c r="N18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O18" s="10" t="s">
+      <c r="N18" t="s">
+        <v>45</v>
+      </c>
+      <c r="O18" t="s">
         <v>230</v>
       </c>
-      <c r="P18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y18" s="10" t="s">
+      <c r="P18" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>45</v>
+      </c>
+      <c r="R18" t="s">
+        <v>45</v>
+      </c>
+      <c r="S18" t="s">
+        <v>45</v>
+      </c>
+      <c r="T18" t="s">
+        <v>45</v>
+      </c>
+      <c r="U18" t="s">
+        <v>45</v>
+      </c>
+      <c r="V18" t="s">
+        <v>45</v>
+      </c>
+      <c r="W18" t="s">
+        <v>45</v>
+      </c>
+      <c r="X18" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y18" t="s">
         <v>46</v>
       </c>
-      <c r="AA18" s="10" t="s">
+      <c r="AA18" t="s">
         <v>48</v>
       </c>
-      <c r="AB18" s="10" t="s">
+      <c r="AB18" t="s">
         <v>48</v>
       </c>
-      <c r="AC18" s="10" t="s">
+      <c r="AC18" t="s">
         <v>57</v>
       </c>
-      <c r="AD18" s="10" t="s">
+      <c r="AD18" t="s">
         <v>48</v>
       </c>
-      <c r="AF18" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG18" s="10" t="s">
+      <c r="AF18" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG18" t="s">
         <v>48</v>
       </c>
-      <c r="AH18" s="10" t="s">
+      <c r="AH18" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>231</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" t="s">
         <v>232</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="D19" t="s">
         <v>233</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" t="s">
         <v>234</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19">
         <v>2000</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19">
         <v>40</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" t="s">
         <v>235</v>
       </c>
-      <c r="J19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K19" s="10" t="s">
+      <c r="J19" t="s">
+        <v>45</v>
+      </c>
+      <c r="K19" t="s">
         <v>236</v>
       </c>
-      <c r="L19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="M19" s="10" t="s">
+      <c r="L19" t="s">
+        <v>45</v>
+      </c>
+      <c r="M19" t="s">
         <v>237</v>
       </c>
-      <c r="N19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O19" s="10" t="s">
+      <c r="N19" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" t="s">
         <v>238</v>
       </c>
-      <c r="P19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y19" s="10" t="s">
+      <c r="P19" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>45</v>
+      </c>
+      <c r="R19" t="s">
+        <v>45</v>
+      </c>
+      <c r="S19" t="s">
+        <v>45</v>
+      </c>
+      <c r="T19" t="s">
+        <v>45</v>
+      </c>
+      <c r="U19" t="s">
+        <v>45</v>
+      </c>
+      <c r="V19" t="s">
+        <v>45</v>
+      </c>
+      <c r="W19" t="s">
+        <v>45</v>
+      </c>
+      <c r="X19" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y19" t="s">
         <v>46</v>
       </c>
-      <c r="AA19" s="10" t="s">
+      <c r="AA19" t="s">
         <v>48</v>
       </c>
-      <c r="AB19" s="10" t="s">
+      <c r="AB19" t="s">
         <v>48</v>
       </c>
-      <c r="AC19" s="10" t="s">
+      <c r="AC19" t="s">
         <v>239</v>
       </c>
-      <c r="AD19" s="10" t="s">
+      <c r="AD19" t="s">
         <v>48</v>
       </c>
-      <c r="AF19" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG19" s="10" t="s">
+      <c r="AF19" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG19" t="s">
         <v>48</v>
       </c>
-      <c r="AH19" s="10" t="s">
+      <c r="AH19" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>240</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="10" t="s">
+      <c r="C20" t="s">
         <v>241</v>
       </c>
-      <c r="D20" s="10" t="s">
+      <c r="D20" t="s">
         <v>242</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" t="s">
         <v>243</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20">
         <v>1952</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20">
         <v>39</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20">
         <v>10</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" t="s">
         <v>244</v>
       </c>
-      <c r="J20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L20" s="10" t="s">
+      <c r="J20" t="s">
+        <v>45</v>
+      </c>
+      <c r="K20" t="s">
+        <v>45</v>
+      </c>
+      <c r="L20" t="s">
         <v>245</v>
       </c>
-      <c r="M20" s="10" t="s">
+      <c r="M20" t="s">
         <v>246</v>
       </c>
-      <c r="N20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" s="10" t="s">
+      <c r="N20" t="s">
+        <v>45</v>
+      </c>
+      <c r="O20" t="s">
         <v>247</v>
       </c>
-      <c r="P20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X20" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y20" s="10" t="s">
+      <c r="P20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>45</v>
+      </c>
+      <c r="R20" t="s">
+        <v>45</v>
+      </c>
+      <c r="S20" t="s">
+        <v>45</v>
+      </c>
+      <c r="T20" t="s">
+        <v>45</v>
+      </c>
+      <c r="U20" t="s">
+        <v>45</v>
+      </c>
+      <c r="V20" t="s">
+        <v>45</v>
+      </c>
+      <c r="W20" t="s">
+        <v>45</v>
+      </c>
+      <c r="X20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y20" t="s">
         <v>46</v>
       </c>
-      <c r="Z20" s="10" t="s">
+      <c r="Z20" t="s">
         <v>86</v>
       </c>
-      <c r="AA20" s="10" t="s">
+      <c r="AA20" t="s">
         <v>48</v>
       </c>
-      <c r="AB20" s="10" t="s">
+      <c r="AB20" t="s">
         <v>48</v>
       </c>
-      <c r="AC20" s="10" t="s">
+      <c r="AC20" t="s">
         <v>248</v>
       </c>
-      <c r="AD20" s="10" t="s">
+      <c r="AD20" t="s">
         <v>48</v>
       </c>
-      <c r="AF20" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG20" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH20" s="10" t="s">
+      <c r="AF20" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>249</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" t="s">
         <v>250</v>
       </c>
-      <c r="D21" s="10" t="s">
+      <c r="D21" t="s">
         <v>251</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" t="s">
         <v>142</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21">
         <v>2003</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21">
         <v>198</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" t="s">
         <v>252</v>
       </c>
-      <c r="J21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="10" t="s">
+      <c r="J21" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" t="s">
         <v>253</v>
       </c>
-      <c r="L21" s="10" t="s">
+      <c r="L21" t="s">
         <v>254</v>
       </c>
-      <c r="M21" s="10" t="s">
+      <c r="M21" t="s">
         <v>146</v>
       </c>
-      <c r="N21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O21" s="10" t="s">
+      <c r="N21" t="s">
+        <v>45</v>
+      </c>
+      <c r="O21" t="s">
         <v>255</v>
       </c>
-      <c r="P21" s="10" t="s">
+      <c r="P21" t="s">
         <v>256</v>
       </c>
-      <c r="Q21" s="10" t="s">
+      <c r="Q21" t="s">
         <v>257</v>
       </c>
-      <c r="R21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X21" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y21" s="10" t="s">
+      <c r="R21" t="s">
+        <v>45</v>
+      </c>
+      <c r="S21" t="s">
+        <v>45</v>
+      </c>
+      <c r="T21" t="s">
+        <v>45</v>
+      </c>
+      <c r="U21" t="s">
+        <v>45</v>
+      </c>
+      <c r="V21" t="s">
+        <v>45</v>
+      </c>
+      <c r="W21" t="s">
+        <v>45</v>
+      </c>
+      <c r="X21" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y21" t="s">
         <v>46</v>
       </c>
-      <c r="AA21" s="10" t="s">
+      <c r="AA21" t="s">
         <v>48</v>
       </c>
-      <c r="AB21" s="10" t="s">
+      <c r="AB21" t="s">
         <v>48</v>
       </c>
-      <c r="AC21" s="10" t="s">
+      <c r="AC21" t="s">
         <v>102</v>
       </c>
-      <c r="AD21" s="10" t="s">
+      <c r="AD21" t="s">
         <v>48</v>
       </c>
-      <c r="AF21" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG21" s="10" t="s">
+      <c r="AF21" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG21" t="s">
         <v>48</v>
       </c>
-      <c r="AH21" s="10" t="s">
+      <c r="AH21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>258</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" t="s">
         <v>259</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" t="s">
         <v>260</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" t="s">
         <v>261</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22">
         <v>2003</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22">
         <v>35</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22">
         <v>2</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" t="s">
         <v>262</v>
       </c>
-      <c r="J22" s="10" t="s">
+      <c r="J22" t="s">
         <v>94</v>
       </c>
-      <c r="K22" s="10" t="s">
+      <c r="K22" t="s">
         <v>263</v>
       </c>
-      <c r="L22" s="10" t="s">
+      <c r="L22" t="s">
         <v>264</v>
       </c>
-      <c r="M22" s="10" t="s">
+      <c r="M22" t="s">
         <v>265</v>
       </c>
-      <c r="N22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O22" s="10" t="s">
+      <c r="N22" t="s">
+        <v>45</v>
+      </c>
+      <c r="O22" t="s">
         <v>266</v>
       </c>
-      <c r="P22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X22" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y22" s="10" t="s">
+      <c r="P22" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>45</v>
+      </c>
+      <c r="R22" t="s">
+        <v>45</v>
+      </c>
+      <c r="S22" t="s">
+        <v>45</v>
+      </c>
+      <c r="T22" t="s">
+        <v>45</v>
+      </c>
+      <c r="U22" t="s">
+        <v>45</v>
+      </c>
+      <c r="V22" t="s">
+        <v>45</v>
+      </c>
+      <c r="W22" t="s">
+        <v>45</v>
+      </c>
+      <c r="X22" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y22" t="s">
         <v>46</v>
       </c>
-      <c r="AA22" s="10" t="s">
+      <c r="AA22" t="s">
         <v>48</v>
       </c>
-      <c r="AB22" s="10" t="s">
+      <c r="AB22" t="s">
         <v>48</v>
       </c>
-      <c r="AC22" s="10" t="s">
+      <c r="AC22" t="s">
         <v>1637</v>
       </c>
-      <c r="AD22" s="10" t="s">
+      <c r="AD22" t="s">
         <v>48</v>
       </c>
-      <c r="AF22" s="10" t="s">
+      <c r="AF22" t="s">
         <v>48</v>
       </c>
-      <c r="AG22" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH22" s="10" t="s">
+      <c r="AG22" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH22" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>267</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" t="s">
         <v>268</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="D23" t="s">
         <v>269</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" t="s">
         <v>270</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23">
         <v>1996</v>
       </c>
-      <c r="G23" s="10">
+      <c r="G23">
         <v>44</v>
       </c>
-      <c r="H23" s="10">
+      <c r="H23">
         <v>4</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I23" t="s">
         <v>271</v>
       </c>
-      <c r="J23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K23" s="10" t="s">
+      <c r="J23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K23" t="s">
         <v>272</v>
       </c>
-      <c r="L23" s="10" t="s">
+      <c r="L23" t="s">
         <v>273</v>
       </c>
-      <c r="M23" s="10" t="s">
+      <c r="M23" t="s">
         <v>274</v>
       </c>
-      <c r="N23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O23" s="10" t="s">
+      <c r="N23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23" t="s">
         <v>275</v>
       </c>
-      <c r="P23" s="10" t="s">
+      <c r="P23" t="s">
         <v>276</v>
       </c>
-      <c r="Q23" s="10" t="s">
+      <c r="Q23" t="s">
         <v>277</v>
       </c>
-      <c r="R23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X23" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y23" s="10" t="s">
+      <c r="R23" t="s">
+        <v>45</v>
+      </c>
+      <c r="S23" t="s">
+        <v>45</v>
+      </c>
+      <c r="T23" t="s">
+        <v>45</v>
+      </c>
+      <c r="U23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V23" t="s">
+        <v>45</v>
+      </c>
+      <c r="W23" t="s">
+        <v>45</v>
+      </c>
+      <c r="X23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y23" t="s">
         <v>46</v>
       </c>
-      <c r="AA23" s="10" t="s">
+      <c r="AA23" t="s">
         <v>48</v>
       </c>
-      <c r="AB23" s="10" t="s">
+      <c r="AB23" t="s">
         <v>48</v>
       </c>
-      <c r="AC23" s="10" t="s">
+      <c r="AC23" t="s">
         <v>278</v>
       </c>
-      <c r="AD23" s="10" t="s">
+      <c r="AD23" t="s">
         <v>48</v>
       </c>
-      <c r="AF23" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG23" s="10" t="s">
+      <c r="AF23" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG23" t="s">
         <v>48</v>
       </c>
-      <c r="AH23" s="10" t="s">
+      <c r="AH23" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>279</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" t="s">
         <v>280</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" t="s">
         <v>281</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" t="s">
         <v>142</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24">
         <v>2000</v>
       </c>
-      <c r="G24" s="10">
+      <c r="G24">
         <v>195</v>
       </c>
-      <c r="H24" s="10">
+      <c r="H24">
         <v>2</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" t="s">
         <v>282</v>
       </c>
-      <c r="J24" s="10" t="s">
+      <c r="J24" t="s">
         <v>283</v>
       </c>
-      <c r="K24" s="10" t="s">
+      <c r="K24" t="s">
         <v>284</v>
       </c>
-      <c r="L24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="M24" s="10" t="s">
+      <c r="L24" t="s">
+        <v>45</v>
+      </c>
+      <c r="M24" t="s">
         <v>146</v>
       </c>
-      <c r="N24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O24" s="10" t="s">
+      <c r="N24" t="s">
+        <v>45</v>
+      </c>
+      <c r="O24" t="s">
         <v>285</v>
       </c>
-      <c r="P24" s="10" t="s">
+      <c r="P24" t="s">
         <v>256</v>
       </c>
-      <c r="Q24" s="10" t="s">
+      <c r="Q24" t="s">
         <v>257</v>
       </c>
-      <c r="R24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X24" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y24" s="10" t="s">
+      <c r="R24" t="s">
+        <v>45</v>
+      </c>
+      <c r="S24" t="s">
+        <v>45</v>
+      </c>
+      <c r="T24" t="s">
+        <v>45</v>
+      </c>
+      <c r="U24" t="s">
+        <v>45</v>
+      </c>
+      <c r="V24" t="s">
+        <v>45</v>
+      </c>
+      <c r="W24" t="s">
+        <v>45</v>
+      </c>
+      <c r="X24" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y24" t="s">
         <v>46</v>
       </c>
-      <c r="Z24" s="10" t="s">
+      <c r="Z24" t="s">
         <v>71</v>
       </c>
-      <c r="AA24" s="10" t="s">
+      <c r="AA24" t="s">
         <v>48</v>
       </c>
-      <c r="AB24" s="10" t="s">
+      <c r="AB24" t="s">
         <v>48</v>
       </c>
-      <c r="AC24" s="10" t="s">
+      <c r="AC24" t="s">
         <v>286</v>
       </c>
-      <c r="AD24" s="10" t="s">
+      <c r="AD24" t="s">
         <v>48</v>
       </c>
-      <c r="AF24" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG24" s="10" t="s">
+      <c r="AF24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG24" t="s">
         <v>48</v>
       </c>
-      <c r="AH24" s="10" t="s">
+      <c r="AH24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>287</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" t="s">
         <v>288</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" t="s">
         <v>289</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" t="s">
         <v>120</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25">
         <v>1998</v>
       </c>
-      <c r="G25" s="10">
+      <c r="G25">
         <v>139</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25">
         <v>3</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" t="s">
         <v>290</v>
       </c>
-      <c r="J25" s="10" t="s">
+      <c r="J25" t="s">
         <v>64</v>
       </c>
-      <c r="K25" s="10" t="s">
+      <c r="K25" t="s">
         <v>291</v>
       </c>
-      <c r="L25" s="10" t="s">
+      <c r="L25" t="s">
         <v>292</v>
       </c>
-      <c r="M25" s="10" t="s">
+      <c r="M25" t="s">
         <v>125</v>
       </c>
-      <c r="N25" s="10" t="s">
+      <c r="N25" t="s">
         <v>136</v>
       </c>
-      <c r="O25" s="10" t="s">
+      <c r="O25" t="s">
         <v>293</v>
       </c>
-      <c r="P25" s="10" t="s">
+      <c r="P25" t="s">
         <v>256</v>
       </c>
-      <c r="Q25" s="10" t="s">
+      <c r="Q25" t="s">
         <v>257</v>
       </c>
-      <c r="R25" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S25" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T25" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U25" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V25" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W25" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X25" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y25" s="10" t="s">
+      <c r="R25" t="s">
+        <v>45</v>
+      </c>
+      <c r="S25" t="s">
+        <v>45</v>
+      </c>
+      <c r="T25" t="s">
+        <v>45</v>
+      </c>
+      <c r="U25" t="s">
+        <v>45</v>
+      </c>
+      <c r="V25" t="s">
+        <v>45</v>
+      </c>
+      <c r="W25" t="s">
+        <v>45</v>
+      </c>
+      <c r="X25" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y25" t="s">
         <v>46</v>
       </c>
-      <c r="AA25" s="10" t="s">
+      <c r="AA25" t="s">
         <v>48</v>
       </c>
-      <c r="AB25" s="10" t="s">
+      <c r="AB25" t="s">
         <v>48</v>
       </c>
-      <c r="AC25" s="10" t="s">
+      <c r="AC25" t="s">
         <v>72</v>
       </c>
-      <c r="AD25" s="10" t="s">
+      <c r="AD25" t="s">
         <v>48</v>
       </c>
-      <c r="AF25" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG25" s="10" t="s">
+      <c r="AF25" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG25" t="s">
         <v>48</v>
       </c>
-      <c r="AH25" s="10" t="s">
+      <c r="AH25" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>294</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" t="s">
         <v>295</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" t="s">
         <v>296</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" t="s">
         <v>120</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26">
         <v>1986</v>
       </c>
-      <c r="G26" s="10">
+      <c r="G26">
         <v>103</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26">
         <v>3</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I26" t="s">
         <v>297</v>
       </c>
-      <c r="J26" s="10" t="s">
+      <c r="J26" t="s">
         <v>64</v>
       </c>
-      <c r="K26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L26" s="10" t="s">
+      <c r="K26" t="s">
+        <v>45</v>
+      </c>
+      <c r="L26" t="s">
         <v>298</v>
       </c>
-      <c r="M26" s="10" t="s">
+      <c r="M26" t="s">
         <v>125</v>
       </c>
-      <c r="N26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O26" s="10" t="s">
+      <c r="N26" t="s">
+        <v>45</v>
+      </c>
+      <c r="O26" t="s">
         <v>299</v>
       </c>
-      <c r="P26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X26" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y26" s="10" t="s">
+      <c r="P26" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>45</v>
+      </c>
+      <c r="R26" t="s">
+        <v>45</v>
+      </c>
+      <c r="S26" t="s">
+        <v>45</v>
+      </c>
+      <c r="T26" t="s">
+        <v>45</v>
+      </c>
+      <c r="U26" t="s">
+        <v>45</v>
+      </c>
+      <c r="V26" t="s">
+        <v>45</v>
+      </c>
+      <c r="W26" t="s">
+        <v>45</v>
+      </c>
+      <c r="X26" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y26" t="s">
         <v>46</v>
       </c>
-      <c r="AA26" s="10" t="s">
+      <c r="AA26" t="s">
         <v>48</v>
       </c>
-      <c r="AB26" s="10" t="s">
+      <c r="AB26" t="s">
         <v>48</v>
       </c>
-      <c r="AC26" s="10" t="s">
+      <c r="AC26" t="s">
         <v>300</v>
       </c>
-      <c r="AD26" s="10" t="s">
+      <c r="AD26" t="s">
         <v>48</v>
       </c>
-      <c r="AF26" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG26" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH26" s="10" t="s">
+      <c r="AF26" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH26" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="27" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>301</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" t="s">
         <v>302</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" t="s">
         <v>303</v>
       </c>
-      <c r="E27" s="10" t="s">
+      <c r="E27" t="s">
         <v>304</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27">
         <v>2006</v>
       </c>
-      <c r="G27" s="10">
+      <c r="G27">
         <v>25</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" t="s">
         <v>305</v>
       </c>
-      <c r="J27" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K27" s="10" t="s">
+      <c r="J27" t="s">
+        <v>45</v>
+      </c>
+      <c r="K27" t="s">
         <v>306</v>
       </c>
-      <c r="L27" s="10" t="s">
+      <c r="L27" t="s">
         <v>307</v>
       </c>
-      <c r="M27" s="10" t="s">
+      <c r="M27" t="s">
         <v>308</v>
       </c>
-      <c r="N27" s="10" t="s">
+      <c r="N27" t="s">
         <v>309</v>
       </c>
-      <c r="O27" s="10" t="s">
+      <c r="O27" t="s">
         <v>310</v>
       </c>
-      <c r="P27" s="10" t="s">
+      <c r="P27" t="s">
         <v>311</v>
       </c>
-      <c r="Q27" s="10" t="s">
+      <c r="Q27" t="s">
         <v>312</v>
       </c>
-      <c r="R27" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S27" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T27" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U27" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V27" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W27" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X27" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y27" s="10" t="s">
+      <c r="R27" t="s">
+        <v>45</v>
+      </c>
+      <c r="S27" t="s">
+        <v>45</v>
+      </c>
+      <c r="T27" t="s">
+        <v>45</v>
+      </c>
+      <c r="U27" t="s">
+        <v>45</v>
+      </c>
+      <c r="V27" t="s">
+        <v>45</v>
+      </c>
+      <c r="W27" t="s">
+        <v>45</v>
+      </c>
+      <c r="X27" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y27" t="s">
         <v>46</v>
       </c>
-      <c r="Z27" s="10" t="s">
+      <c r="Z27" t="s">
         <v>47</v>
       </c>
-      <c r="AA27" s="10" t="s">
+      <c r="AA27" t="s">
         <v>48</v>
       </c>
-      <c r="AB27" s="10" t="s">
+      <c r="AB27" t="s">
         <v>48</v>
       </c>
-      <c r="AC27" s="10" t="s">
+      <c r="AC27" t="s">
         <v>313</v>
       </c>
-      <c r="AD27" s="10" t="s">
+      <c r="AD27" t="s">
         <v>48</v>
       </c>
-      <c r="AF27" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG27" s="10" t="s">
+      <c r="AF27" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG27" t="s">
         <v>48</v>
       </c>
-      <c r="AH27" s="10" t="s">
+      <c r="AH27" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>314</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" t="s">
         <v>315</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" t="s">
         <v>316</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" t="s">
         <v>317</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28">
         <v>1985</v>
       </c>
-      <c r="G28" s="10">
+      <c r="G28">
         <v>98</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28">
         <v>1049</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I28" t="s">
         <v>318</v>
       </c>
-      <c r="J28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L28" s="10" t="s">
+      <c r="J28" t="s">
+        <v>45</v>
+      </c>
+      <c r="K28" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28" t="s">
         <v>319</v>
       </c>
-      <c r="M28" s="10" t="s">
+      <c r="M28" t="s">
         <v>320</v>
       </c>
-      <c r="N28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O28" s="10" t="s">
+      <c r="N28" t="s">
+        <v>45</v>
+      </c>
+      <c r="O28" t="s">
         <v>321</v>
       </c>
-      <c r="P28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X28" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y28" s="10" t="s">
+      <c r="P28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>45</v>
+      </c>
+      <c r="R28" t="s">
+        <v>45</v>
+      </c>
+      <c r="S28" t="s">
+        <v>45</v>
+      </c>
+      <c r="T28" t="s">
+        <v>45</v>
+      </c>
+      <c r="U28" t="s">
+        <v>45</v>
+      </c>
+      <c r="V28" t="s">
+        <v>45</v>
+      </c>
+      <c r="W28" t="s">
+        <v>45</v>
+      </c>
+      <c r="X28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y28" t="s">
         <v>46</v>
       </c>
-      <c r="AA28" s="10" t="s">
+      <c r="AA28" t="s">
         <v>48</v>
       </c>
-      <c r="AB28" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AC28" s="10" t="s">
+      <c r="AB28" t="s">
+        <v>116</v>
+      </c>
+      <c r="AC28" t="s">
         <v>1632</v>
       </c>
-      <c r="AD28" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AE28" s="10" t="s">
+      <c r="AD28" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE28" t="s">
         <v>1638</v>
       </c>
     </row>
-    <row r="29" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>322</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" t="s">
         <v>280</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D29" t="s">
         <v>323</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" t="s">
         <v>261</v>
       </c>
-      <c r="F29" s="10">
+      <c r="F29">
         <v>2004</v>
       </c>
-      <c r="G29" s="10">
+      <c r="G29">
         <v>36</v>
       </c>
-      <c r="H29" s="10">
+      <c r="H29">
         <v>5</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I29" t="s">
         <v>324</v>
       </c>
-      <c r="J29" s="10" t="s">
+      <c r="J29" t="s">
         <v>175</v>
       </c>
-      <c r="K29" s="10" t="s">
+      <c r="K29" t="s">
         <v>325</v>
       </c>
-      <c r="L29" s="10" t="s">
+      <c r="L29" t="s">
         <v>326</v>
       </c>
-      <c r="M29" s="10" t="s">
+      <c r="M29" t="s">
         <v>265</v>
       </c>
-      <c r="N29" s="10" t="s">
+      <c r="N29" t="s">
         <v>327</v>
       </c>
-      <c r="O29" s="10" t="s">
+      <c r="O29" t="s">
         <v>328</v>
       </c>
-      <c r="P29" s="10" t="s">
+      <c r="P29" t="s">
         <v>256</v>
       </c>
-      <c r="Q29" s="10" t="s">
+      <c r="Q29" t="s">
         <v>257</v>
       </c>
-      <c r="R29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X29" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y29" s="10" t="s">
+      <c r="R29" t="s">
+        <v>45</v>
+      </c>
+      <c r="S29" t="s">
+        <v>45</v>
+      </c>
+      <c r="T29" t="s">
+        <v>45</v>
+      </c>
+      <c r="U29" t="s">
+        <v>45</v>
+      </c>
+      <c r="V29" t="s">
+        <v>45</v>
+      </c>
+      <c r="W29" t="s">
+        <v>45</v>
+      </c>
+      <c r="X29" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y29" t="s">
         <v>46</v>
       </c>
-      <c r="AA29" s="10" t="s">
+      <c r="AA29" t="s">
         <v>48</v>
       </c>
-      <c r="AB29" s="10" t="s">
+      <c r="AB29" t="s">
         <v>48</v>
       </c>
-      <c r="AC29" s="10" t="s">
+      <c r="AC29" t="s">
         <v>329</v>
       </c>
-      <c r="AD29" s="10" t="s">
+      <c r="AD29" t="s">
         <v>48</v>
       </c>
-      <c r="AF29" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG29" s="10" t="s">
+      <c r="AF29" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG29" t="s">
         <v>48</v>
       </c>
-      <c r="AH29" s="10" t="s">
+      <c r="AH29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>330</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="10" t="s">
+      <c r="C30" t="s">
         <v>331</v>
       </c>
-      <c r="D30" s="10" t="s">
+      <c r="D30" t="s">
         <v>332</v>
       </c>
-      <c r="E30" s="10" t="s">
+      <c r="E30" t="s">
         <v>261</v>
       </c>
-      <c r="F30" s="10">
+      <c r="F30">
         <v>1997</v>
       </c>
-      <c r="G30" s="10">
+      <c r="G30">
         <v>29</v>
       </c>
-      <c r="H30" s="10">
+      <c r="H30">
         <v>1</v>
       </c>
-      <c r="I30" s="10" t="s">
+      <c r="I30" t="s">
         <v>333</v>
       </c>
-      <c r="J30" s="10" t="s">
+      <c r="J30" t="s">
         <v>52</v>
       </c>
-      <c r="K30" s="10" t="s">
+      <c r="K30" t="s">
         <v>334</v>
       </c>
-      <c r="L30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="M30" s="10" t="s">
+      <c r="L30" t="s">
+        <v>45</v>
+      </c>
+      <c r="M30" t="s">
         <v>265</v>
       </c>
-      <c r="N30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O30" s="10" t="s">
+      <c r="N30" t="s">
+        <v>45</v>
+      </c>
+      <c r="O30" t="s">
         <v>335</v>
       </c>
-      <c r="P30" s="10" t="s">
+      <c r="P30" t="s">
         <v>336</v>
       </c>
-      <c r="Q30" s="10" t="s">
+      <c r="Q30" t="s">
         <v>337</v>
       </c>
-      <c r="R30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X30" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y30" s="10" t="s">
+      <c r="R30" t="s">
+        <v>45</v>
+      </c>
+      <c r="S30" t="s">
+        <v>45</v>
+      </c>
+      <c r="T30" t="s">
+        <v>45</v>
+      </c>
+      <c r="U30" t="s">
+        <v>45</v>
+      </c>
+      <c r="V30" t="s">
+        <v>45</v>
+      </c>
+      <c r="W30" t="s">
+        <v>45</v>
+      </c>
+      <c r="X30" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y30" t="s">
         <v>46</v>
       </c>
-      <c r="AA30" s="10" t="s">
+      <c r="AA30" t="s">
         <v>48</v>
       </c>
-      <c r="AB30" s="10" t="s">
+      <c r="AB30" t="s">
         <v>48</v>
       </c>
-      <c r="AC30" s="10" t="s">
+      <c r="AC30" t="s">
         <v>57</v>
       </c>
-      <c r="AD30" s="10" t="s">
+      <c r="AD30" t="s">
         <v>48</v>
       </c>
-      <c r="AF30" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG30" s="10" t="s">
+      <c r="AF30" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG30" t="s">
         <v>48</v>
       </c>
-      <c r="AH30" s="10" t="s">
+      <c r="AH30" t="s">
         <v>48</v>
       </c>
     </row>
@@ -12044,101 +12045,101 @@
         <v>710</v>
       </c>
     </row>
-    <row r="67" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="10" t="s">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>711</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B67" t="s">
         <v>32</v>
       </c>
-      <c r="C67" s="10" t="s">
+      <c r="C67" t="s">
         <v>712</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="D67" t="s">
         <v>713</v>
       </c>
-      <c r="E67" s="10" t="s">
+      <c r="E67" t="s">
         <v>35</v>
       </c>
-      <c r="F67" s="10">
+      <c r="F67">
         <v>1980</v>
       </c>
-      <c r="G67" s="10">
-        <v>45</v>
-      </c>
-      <c r="H67" s="10">
+      <c r="G67">
+        <v>45</v>
+      </c>
+      <c r="H67">
         <v>1</v>
       </c>
-      <c r="I67" s="10" t="s">
+      <c r="I67" t="s">
         <v>714</v>
       </c>
-      <c r="J67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="L67" s="10" t="s">
+      <c r="J67" t="s">
+        <v>45</v>
+      </c>
+      <c r="K67" t="s">
+        <v>45</v>
+      </c>
+      <c r="L67" t="s">
         <v>715</v>
       </c>
-      <c r="M67" s="10" t="s">
+      <c r="M67" t="s">
         <v>40</v>
       </c>
-      <c r="N67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="O67" s="10" t="s">
+      <c r="N67" t="s">
+        <v>45</v>
+      </c>
+      <c r="O67" t="s">
         <v>716</v>
       </c>
-      <c r="P67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X67" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y67" s="10" t="s">
+      <c r="P67" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q67" t="s">
+        <v>45</v>
+      </c>
+      <c r="R67" t="s">
+        <v>45</v>
+      </c>
+      <c r="S67" t="s">
+        <v>45</v>
+      </c>
+      <c r="T67" t="s">
+        <v>45</v>
+      </c>
+      <c r="U67" t="s">
+        <v>45</v>
+      </c>
+      <c r="V67" t="s">
+        <v>45</v>
+      </c>
+      <c r="W67" t="s">
+        <v>45</v>
+      </c>
+      <c r="X67" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y67" t="s">
         <v>46</v>
       </c>
-      <c r="AA67" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AB67" s="10" t="s">
+      <c r="AA67" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB67" t="s">
         <v>48</v>
       </c>
-      <c r="AC67" s="10" t="s">
+      <c r="AC67" t="s">
         <v>72</v>
       </c>
-      <c r="AD67" s="10" t="s">
+      <c r="AD67" t="s">
         <v>48</v>
       </c>
-      <c r="AF67" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG67" s="10" t="s">
+      <c r="AF67" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG67" t="s">
         <v>48</v>
       </c>
-      <c r="AH67" s="10" t="s">
+      <c r="AH67" t="s">
         <v>48</v>
       </c>
     </row>
@@ -19476,101 +19477,101 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="153" spans="1:34" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A153" s="10" t="s">
+    <row r="153" spans="1:34" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
         <v>1574</v>
       </c>
-      <c r="B153" s="10" t="s">
+      <c r="B153" t="s">
         <v>32</v>
       </c>
-      <c r="C153" s="10" t="s">
+      <c r="C153" t="s">
         <v>1575</v>
       </c>
-      <c r="D153" s="10" t="s">
+      <c r="D153" t="s">
         <v>1576</v>
       </c>
-      <c r="E153" s="10" t="s">
+      <c r="E153" t="s">
         <v>142</v>
       </c>
-      <c r="F153" s="10">
+      <c r="F153">
         <v>1991</v>
       </c>
-      <c r="G153" s="10">
+      <c r="G153">
         <v>185</v>
       </c>
-      <c r="H153" s="10">
+      <c r="H153">
         <v>3</v>
       </c>
-      <c r="I153" s="10" t="s">
+      <c r="I153" t="s">
         <v>1577</v>
       </c>
-      <c r="J153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K153" s="10" t="s">
+      <c r="J153" t="s">
+        <v>45</v>
+      </c>
+      <c r="K153" t="s">
         <v>1578</v>
       </c>
-      <c r="L153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="M153" s="10" t="s">
+      <c r="L153" t="s">
+        <v>45</v>
+      </c>
+      <c r="M153" t="s">
         <v>146</v>
       </c>
-      <c r="N153" s="10" t="s">
+      <c r="N153" t="s">
         <v>147</v>
       </c>
-      <c r="O153" s="10" t="s">
+      <c r="O153" t="s">
         <v>1579</v>
       </c>
-      <c r="P153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="R153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="S153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="T153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="U153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="V153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="W153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X153" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y153" s="10" t="s">
+      <c r="P153" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q153" t="s">
+        <v>45</v>
+      </c>
+      <c r="R153" t="s">
+        <v>45</v>
+      </c>
+      <c r="S153" t="s">
+        <v>45</v>
+      </c>
+      <c r="T153" t="s">
+        <v>45</v>
+      </c>
+      <c r="U153" t="s">
+        <v>45</v>
+      </c>
+      <c r="V153" t="s">
+        <v>45</v>
+      </c>
+      <c r="W153" t="s">
+        <v>45</v>
+      </c>
+      <c r="X153" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y153" t="s">
         <v>46</v>
       </c>
-      <c r="Z153" s="10" t="s">
+      <c r="Z153" t="s">
         <v>1634</v>
       </c>
-      <c r="AA153" s="10" t="s">
+      <c r="AA153" t="s">
         <v>48</v>
       </c>
-      <c r="AB153" s="10" t="s">
+      <c r="AB153" t="s">
         <v>48</v>
       </c>
-      <c r="AE153" s="10" t="s">
+      <c r="AE153" t="s">
         <v>1635</v>
       </c>
-      <c r="AF153" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="AG153" s="10" t="s">
+      <c r="AF153" t="s">
+        <v>116</v>
+      </c>
+      <c r="AG153" t="s">
         <v>48</v>
       </c>
-      <c r="AH153" s="10" t="s">
+      <c r="AH153" t="s">
         <v>48</v>
       </c>
     </row>
@@ -19841,8 +19842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123BDFED-BA12-FF4C-8CED-29BDD290375F}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19945,6 +19946,9 @@
       </c>
       <c r="B5" t="s">
         <v>1647</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1667</v>
       </c>
       <c r="D5" t="s">
         <v>1648</v>

</xml_diff>